<commit_message>
corridor comparison table excel sheet
</commit_message>
<xml_diff>
--- a/Memo/corridor_comparison_table.xlsx
+++ b/Memo/corridor_comparison_table.xlsx
@@ -13,6 +13,7 @@
   </bookViews>
   <sheets>
     <sheet name="Minneapolis" sheetId="1" r:id="rId1"/>
+    <sheet name="Indianapolis" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="28">
   <si>
     <t>Control Corridor</t>
   </si>
@@ -93,6 +94,21 @@
   </si>
   <si>
     <t>û</t>
+  </si>
+  <si>
+    <t>Virginia</t>
+  </si>
+  <si>
+    <t>Meridian</t>
+  </si>
+  <si>
+    <t>Prospect</t>
+  </si>
+  <si>
+    <t>Shelby</t>
+  </si>
+  <si>
+    <t>Mass Ave.</t>
   </si>
 </sst>
 </file>
@@ -129,7 +145,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -178,17 +194,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -212,6 +242,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -506,230 +542,230 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="4" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="6" t="s">
+      <c r="C1" s="6"/>
+      <c r="D1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="E1" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="H1" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="6" t="s">
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="12" t="s">
+      <c r="C3" s="12"/>
+      <c r="D3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" s="12" t="s">
+      <c r="F3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="9"/>
-      <c r="B4" s="10" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F4" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G4" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="12" t="s">
+      <c r="C4" s="12"/>
+      <c r="D4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="9"/>
-      <c r="B5" s="10" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H5" s="12" t="s">
+      <c r="C5" s="12"/>
+      <c r="D5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D6" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G6" s="12" t="s">
+      <c r="D6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G6" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H6" s="12" t="s">
+      <c r="H6" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="6" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F7" s="12" t="s">
+      <c r="E7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="12" t="s">
+      <c r="H7" s="13" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11" t="s">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H8" s="12" t="s">
+      <c r="C8" s="12"/>
+      <c r="D8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10" t="s">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="12" t="s">
+      <c r="D9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10"/>
-      <c r="C10" s="6" t="s">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="G10" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="H10" s="12" t="s">
+      <c r="D10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" s="13" t="s">
         <v>21</v>
       </c>
     </row>
@@ -749,4 +785,231 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
+    <col min="3" max="3" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="4"/>
+      <c r="B1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="15"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="10"/>
+      <c r="B4" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="12"/>
+      <c r="D4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="10"/>
+      <c r="B5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="12"/>
+      <c r="D5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="11"/>
+      <c r="B8" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="11"/>
+      <c r="B9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="11"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="G10" s="13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A6:A10"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="A3:A5"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B5:C5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>